<commit_message>
validation and updates to the core forge model
Okay, this is the big update. I fixed (as much as I could) the issues surrounding the sponsorship and committees. There's a small number of bills that are competitive and an even smaller number that we have committee data for (part of that seems to be time-related, Legiscan doesn't have reliable committee data for the older sessions). All of the outputs are now generated and saved out, I've regenerated the histograms and everything should be hunky-dory. The next step is to take these outputs and actually do the model with Bayesian updating.
</commit_message>
<xml_diff>
--- a/outputs/house_democrats_chamber_sponsor.xlsx
+++ b/outputs/house_democrats_chamber_sponsor.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="6660"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14415" windowHeight="10080"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -519,40 +519,40 @@
         <v>11</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="G2">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="H2">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="I2">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="J2">
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="K2">
-        <v>1</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="L2">
-        <v>1</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="M2">
-        <v>1</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -560,37 +560,37 @@
         <v>12</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="F3">
         <v>1</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="H3">
-        <v>1</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="K3">
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="L3">
-        <v>1</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="M3">
         <v>1</v>
@@ -600,22 +600,49 @@
       <c r="A4" t="s">
         <v>13</v>
       </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="F5">
         <v>1</v>
@@ -626,14 +653,20 @@
       <c r="H5">
         <v>1</v>
       </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
       <c r="J5">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="K5">
-        <v>1</v>
+        <v>0.5</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
       </c>
       <c r="M5">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -641,34 +674,37 @@
         <v>15</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="E6">
-        <v>1</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="F6">
         <v>1</v>
       </c>
       <c r="G6">
-        <v>1</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="H6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="I6">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J6">
-        <v>1</v>
+        <v>0.75</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
       </c>
       <c r="L6">
-        <v>1</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="M6">
         <v>1</v>
@@ -693,6 +729,12 @@
       <c r="F7">
         <v>1</v>
       </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
       <c r="I7">
         <v>1</v>
       </c>
@@ -701,6 +743,9 @@
       </c>
       <c r="K7">
         <v>1</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
       </c>
       <c r="M7">
         <v>1</v>
@@ -710,15 +755,24 @@
       <c r="A8" t="s">
         <v>17</v>
       </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
       <c r="C8">
         <v>1</v>
       </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
       <c r="E8">
         <v>1</v>
       </c>
       <c r="F8">
         <v>1</v>
       </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
       <c r="H8">
         <v>1</v>
       </c>
@@ -727,6 +781,9 @@
       </c>
       <c r="J8">
         <v>1</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
       </c>
       <c r="L8">
         <v>1</v>
@@ -740,40 +797,40 @@
         <v>1</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>0.4375</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>0.38461538461538464</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="E9">
-        <v>1</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="F9">
-        <v>1</v>
+        <v>0.8125</v>
       </c>
       <c r="G9">
-        <v>1</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="H9">
-        <v>1</v>
+        <v>0.625</v>
       </c>
       <c r="I9">
-        <v>1</v>
+        <v>0.4375</v>
       </c>
       <c r="J9">
-        <v>1</v>
+        <v>0.625</v>
       </c>
       <c r="K9">
-        <v>1</v>
+        <v>0.2857142857142857</v>
       </c>
       <c r="L9">
-        <v>1</v>
+        <v>0.7142857142857143</v>
       </c>
       <c r="M9">
-        <v>1</v>
+        <v>0.53333333333333333</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -799,7 +856,7 @@
         <v>1</v>
       </c>
       <c r="H10">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="I10">
         <v>1</v>
@@ -818,20 +875,41 @@
       <c r="A11" t="s">
         <v>19</v>
       </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
       <c r="C11">
-        <v>1</v>
+        <v>0.5</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
       </c>
       <c r="F11">
-        <v>1</v>
+        <v>0.5</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
       </c>
       <c r="H11">
-        <v>1</v>
+        <v>0.5</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
       </c>
       <c r="J11">
-        <v>1</v>
+        <v>0.5</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
       </c>
       <c r="M11">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -839,40 +917,40 @@
         <v>2</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="E12">
-        <v>1</v>
+        <v>0.5714285714285714</v>
       </c>
       <c r="F12">
-        <v>1</v>
+        <v>0.7142857142857143</v>
       </c>
       <c r="G12">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="H12">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="I12">
-        <v>1</v>
+        <v>0.42857142857142855</v>
       </c>
       <c r="J12">
-        <v>1</v>
+        <v>0.42857142857142855</v>
       </c>
       <c r="K12">
-        <v>1</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="L12">
         <v>1</v>
       </c>
       <c r="M12">
-        <v>1</v>
+        <v>0.8571428571428571</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -880,40 +958,40 @@
         <v>3</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="D13">
         <v>1</v>
       </c>
       <c r="E13">
-        <v>1</v>
+        <v>0.875</v>
       </c>
       <c r="F13">
         <v>1</v>
       </c>
       <c r="G13">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="H13">
-        <v>1</v>
+        <v>0.625</v>
       </c>
       <c r="I13">
-        <v>1</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="J13">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="K13">
-        <v>1</v>
+        <v>0.55555555555555558</v>
       </c>
       <c r="L13">
-        <v>1</v>
+        <v>0.88888888888888884</v>
       </c>
       <c r="M13">
-        <v>1</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -921,13 +999,13 @@
         <v>4</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>0.7142857142857143</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="D14">
-        <v>1</v>
+        <v>0.7142857142857143</v>
       </c>
       <c r="E14">
         <v>1</v>
@@ -936,25 +1014,25 @@
         <v>1</v>
       </c>
       <c r="G14">
-        <v>1</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="H14">
-        <v>1</v>
+        <v>0.5714285714285714</v>
       </c>
       <c r="I14">
         <v>1</v>
       </c>
       <c r="J14">
-        <v>1</v>
+        <v>0.5714285714285714</v>
       </c>
       <c r="K14">
-        <v>1</v>
+        <v>0.7142857142857143</v>
       </c>
       <c r="L14">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="M14">
-        <v>1</v>
+        <v>0.8571428571428571</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -962,40 +1040,40 @@
         <v>5</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="D15">
         <v>1</v>
       </c>
       <c r="E15">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="F15">
         <v>1</v>
       </c>
       <c r="G15">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="H15">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="I15">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="J15">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="K15">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="L15">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="M15">
-        <v>1</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -1003,37 +1081,40 @@
         <v>6</v>
       </c>
       <c r="B16">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="C16">
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="D16">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="E16">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="F16">
-        <v>1</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="G16">
-        <v>1</v>
+        <v>0.8</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
       </c>
       <c r="I16">
-        <v>1</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="J16">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="K16">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="L16">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="M16">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
@@ -1059,16 +1140,19 @@
         <v>1</v>
       </c>
       <c r="H17">
-        <v>1</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="I17">
         <v>1</v>
       </c>
       <c r="J17">
-        <v>1</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="K17">
         <v>1</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
       </c>
       <c r="M17">
         <v>1</v>
@@ -1079,40 +1163,40 @@
         <v>7</v>
       </c>
       <c r="B18">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="C18">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="D18">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="E18">
-        <v>1</v>
+        <v>0.3</v>
       </c>
       <c r="F18">
         <v>1</v>
       </c>
       <c r="G18">
-        <v>1</v>
+        <v>0.22222222222222221</v>
       </c>
       <c r="H18">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="I18">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J18">
-        <v>1</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="K18">
-        <v>1</v>
+        <v>0.22222222222222221</v>
       </c>
       <c r="L18">
         <v>1</v>
       </c>
       <c r="M18">
-        <v>1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
@@ -1120,7 +1204,7 @@
         <v>21</v>
       </c>
       <c r="B19">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D19">
         <v>1</v>
@@ -1134,20 +1218,23 @@
       <c r="G19">
         <v>1</v>
       </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
       <c r="I19">
         <v>1</v>
       </c>
       <c r="J19">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="K19">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="L19">
         <v>1</v>
       </c>
       <c r="M19">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
@@ -1155,7 +1242,7 @@
         <v>22</v>
       </c>
       <c r="B20">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -1169,20 +1256,23 @@
       <c r="G20">
         <v>1</v>
       </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
       <c r="I20">
         <v>1</v>
       </c>
       <c r="J20">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="K20">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="L20">
         <v>1</v>
       </c>
       <c r="M20">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
@@ -1190,37 +1280,40 @@
         <v>8</v>
       </c>
       <c r="B21">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="C21">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="D21">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="E21">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="F21">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="G21">
-        <v>1</v>
+        <v>0.5</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
       </c>
       <c r="I21">
-        <v>1</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="J21">
-        <v>1</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="K21">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="L21">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="M21">
-        <v>1</v>
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
@@ -1228,31 +1321,34 @@
         <v>23</v>
       </c>
       <c r="B22">
-        <v>1</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="C22">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D22">
-        <v>1</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="E22">
-        <v>1</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="F22">
         <v>1</v>
       </c>
       <c r="G22">
-        <v>1</v>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
       </c>
       <c r="I22">
         <v>1</v>
       </c>
       <c r="J22">
-        <v>1</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="K22">
-        <v>1</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="L22">
         <v>1</v>
@@ -1266,13 +1362,13 @@
         <v>24</v>
       </c>
       <c r="B23">
-        <v>1</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="C23">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D23">
-        <v>1</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="E23">
         <v>1</v>
@@ -1281,16 +1377,19 @@
         <v>1</v>
       </c>
       <c r="G23">
-        <v>1</v>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
       </c>
       <c r="I23">
-        <v>1</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="J23">
-        <v>1</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="K23">
-        <v>1</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="M23">
         <v>1</v>
@@ -1319,7 +1418,7 @@
         <v>1</v>
       </c>
       <c r="H24">
-        <v>1</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="I24">
         <v>1</v>
@@ -1356,6 +1455,12 @@
       <c r="F25">
         <v>1</v>
       </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
       <c r="I25">
         <v>1</v>
       </c>
@@ -1373,17 +1478,41 @@
       <c r="A26" t="s">
         <v>27</v>
       </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
       <c r="E26">
-        <v>1</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="F26">
-        <v>1</v>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
       </c>
       <c r="H26">
-        <v>1</v>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <v>0</v>
+      </c>
+      <c r="K26">
+        <v>0</v>
       </c>
       <c r="L26">
-        <v>1</v>
+        <v>0.5</v>
+      </c>
+      <c r="M26">
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
@@ -1391,40 +1520,40 @@
         <v>9</v>
       </c>
       <c r="B27">
-        <v>0.75</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="C27">
-        <v>0.83333333333333337</v>
+        <v>0.45454545454545453</v>
       </c>
       <c r="D27">
-        <v>0.75</v>
+        <v>0.27272727272727271</v>
       </c>
       <c r="E27">
-        <v>0.75</v>
+        <v>0.27272727272727271</v>
       </c>
       <c r="F27">
-        <v>0.88888888888888884</v>
+        <v>0.72727272727272729</v>
       </c>
       <c r="G27">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="H27">
-        <v>0.875</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="I27">
-        <v>0.8</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="J27">
-        <v>0.875</v>
+        <v>0.63636363636363635</v>
       </c>
       <c r="K27">
-        <v>0.66666666666666663</v>
+        <v>0.18181818181818182</v>
       </c>
       <c r="L27">
-        <v>0.8571428571428571</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="M27">
-        <v>0.875</v>
+        <v>0.58333333333333337</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
@@ -1432,40 +1561,40 @@
         <v>10</v>
       </c>
       <c r="B28">
-        <v>1</v>
+        <v>0.375</v>
       </c>
       <c r="C28">
-        <v>1</v>
+        <v>0.625</v>
       </c>
       <c r="D28">
-        <v>1</v>
+        <v>0.375</v>
       </c>
       <c r="E28">
-        <v>1</v>
+        <v>0.375</v>
       </c>
       <c r="F28">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="G28">
-        <v>1</v>
+        <v>0.14285714285714285</v>
       </c>
       <c r="H28">
-        <v>1</v>
+        <v>0.2857142857142857</v>
       </c>
       <c r="I28">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="J28">
-        <v>1</v>
+        <v>0.42857142857142855</v>
       </c>
       <c r="K28">
-        <v>1</v>
+        <v>0.625</v>
       </c>
       <c r="L28">
-        <v>1</v>
+        <v>0.5714285714285714</v>
       </c>
       <c r="M28">
-        <v>1</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
@@ -1473,40 +1602,40 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>1</v>
+        <v>0.375</v>
       </c>
       <c r="C29">
-        <v>1</v>
+        <v>0.7142857142857143</v>
       </c>
       <c r="D29">
-        <v>1</v>
+        <v>0.625</v>
       </c>
       <c r="E29">
-        <v>1</v>
+        <v>0.5714285714285714</v>
       </c>
       <c r="F29">
-        <v>1</v>
+        <v>0.7142857142857143</v>
       </c>
       <c r="G29">
-        <v>1</v>
+        <v>0.42857142857142855</v>
       </c>
       <c r="H29">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="I29">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J29">
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="K29">
-        <v>1</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="L29">
         <v>1</v>
       </c>
       <c r="M29">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
@@ -1517,31 +1646,31 @@
         <v>1</v>
       </c>
       <c r="C30">
-        <v>1</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="D30">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="E30">
         <v>1</v>
       </c>
       <c r="F30">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="G30">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="H30">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="I30">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="J30">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="K30">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="L30">
         <v>1</v>

</xml_diff>